<commit_message>
proprocessing weather and city data
</commit_message>
<xml_diff>
--- a/docs/metadata.xlsx
+++ b/docs/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simof\Documents\GitHub\thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B29980F-22F3-4348-97A0-1BBBBD757D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D290E-840E-4DAA-980A-F64F02AA8A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0FD02F1D-79EF-43F7-86ED-8D794E1915BF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="351">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -1055,6 +1055,39 @@
   </si>
   <si>
     <t>Classe di rilevazione</t>
+  </si>
+  <si>
+    <t>Fascia demografica</t>
+  </si>
+  <si>
+    <t>Classe ordinale</t>
+  </si>
+  <si>
+    <t>0 -&gt; 6</t>
+  </si>
+  <si>
+    <t>&lt;1k, 1k-5k, 5k-10k, 10k-50k, 50k-100k, 100k-250k, &gt;250k</t>
+  </si>
+  <si>
+    <t>Grado di urbanizzazione</t>
+  </si>
+  <si>
+    <t>Vclasse ordinale</t>
+  </si>
+  <si>
+    <t>0 -&gt; 2</t>
+  </si>
+  <si>
+    <t>zone rurali, piccola città e sobborghi, città</t>
+  </si>
+  <si>
+    <t>IFC (valori)</t>
+  </si>
+  <si>
+    <t>0 -&gt; 9</t>
+  </si>
+  <si>
+    <t>0 -&gt; 16</t>
   </si>
 </sst>
 </file>
@@ -1123,12 +1156,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1139,24 +1171,6 @@
     <cellStyle name="Normale 2" xfId="1" xr:uid="{8E5D2C1A-2E4B-48ED-AAFF-918A1143607F}"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1220,6 +1234,24 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1234,7 +1266,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDDE8B1E-BC8E-4AEB-94B6-6E3F9E8A29B0}" name="Tabella10" displayName="Tabella10" ref="A1:D29" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDDE8B1E-BC8E-4AEB-94B6-6E3F9E8A29B0}" name="Tabella10" displayName="Tabella10" ref="A1:D29" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:D29" xr:uid="{CDDE8B1E-BC8E-4AEB-94B6-6E3F9E8A29B0}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C052614B-1417-427E-ABBE-FD86E7706423}" name="VARIABLE"/>
@@ -1247,7 +1279,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{62E8A6FA-6F99-4C6B-A379-78C951518DBD}" name="Tabella2" displayName="Tabella2" ref="A1:D11" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{62E8A6FA-6F99-4C6B-A379-78C951518DBD}" name="Tabella2" displayName="Tabella2" ref="A1:D11" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:D11" xr:uid="{62E8A6FA-6F99-4C6B-A379-78C951518DBD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{24548C0D-A35B-47A8-9DC4-A446EA90AFB5}" name="VARIABLE"/>
@@ -1260,7 +1292,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1C4613CA-2DAA-4DD4-A8B4-B7A01CD0F8CB}" name="Tabella9" displayName="Tabella9" ref="A1:C45" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1C4613CA-2DAA-4DD4-A8B4-B7A01CD0F8CB}" name="Tabella9" displayName="Tabella9" ref="A1:C45" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:C45" xr:uid="{1C4613CA-2DAA-4DD4-A8B4-B7A01CD0F8CB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C7EC7D0C-8B5A-4A01-9E9F-F36A4E681114}" name="VARIABLE"/>
@@ -1272,10 +1304,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A559DF72-5DDE-418B-9DD5-19E9315919C2}" name="Tabella8" displayName="Tabella8" ref="A1:C9" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A559DF72-5DDE-418B-9DD5-19E9315919C2}" name="Tabella8" displayName="Tabella8" ref="A1:C9" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:C9" xr:uid="{A559DF72-5DDE-418B-9DD5-19E9315919C2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E8749555-B9F8-4941-8B82-3ED92020DA1B}" name="VARIABLE" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E8749555-B9F8-4941-8B82-3ED92020DA1B}" name="VARIABLE" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{D96A4B11-5E19-4B4F-90ED-A857C12A9C5B}" name="UNIT OF MEASURE"/>
     <tableColumn id="3" xr3:uid="{3EA4292B-BBE8-42AC-856D-9A3DB2DE3BB0}" name="DESCRIPTION"/>
   </tableColumns>
@@ -1284,7 +1316,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A495E3D1-7E8D-4F8F-85F6-490434CDC856}" name="Tabella7" displayName="Tabella7" ref="A1:C46" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A495E3D1-7E8D-4F8F-85F6-490434CDC856}" name="Tabella7" displayName="Tabella7" ref="A1:C46" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:C46" xr:uid="{A495E3D1-7E8D-4F8F-85F6-490434CDC856}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1618CB93-2EF2-4C57-AB33-FCDF160AE2B8}" name="VARIABLE"/>
@@ -1296,7 +1328,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9CD07A7C-A0B2-46E1-93CE-F310E76C584A}" name="Tabella6" displayName="Tabella6" ref="A1:C40" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9CD07A7C-A0B2-46E1-93CE-F310E76C584A}" name="Tabella6" displayName="Tabella6" ref="A1:C40" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:C40" xr:uid="{9CD07A7C-A0B2-46E1-93CE-F310E76C584A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{702A4E55-DC8F-4477-8E3D-0311045AB7EA}" name="VARIABLE"/>
@@ -1308,7 +1340,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8EBA25E5-8C91-4969-98D3-F0280C56705F}" name="Tabella5" displayName="Tabella5" ref="A1:D28" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8EBA25E5-8C91-4969-98D3-F0280C56705F}" name="Tabella5" displayName="Tabella5" ref="A1:D28" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:D28" xr:uid="{8EBA25E5-8C91-4969-98D3-F0280C56705F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0BE9B6DA-8EC3-436E-AF25-0891DF98A195}" name="VARIABLE"/>
@@ -1321,34 +1353,34 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EB0DE39-C134-4496-8DF4-B7B7CD2384B8}" name="Tabella3" displayName="Tabella3" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EB0DE39-C134-4496-8DF4-B7B7CD2384B8}" name="Tabella3" displayName="Tabella3" ref="A1:D9" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D9" xr:uid="{2EB0DE39-C134-4496-8DF4-B7B7CD2384B8}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E731BF0C-6DEC-4FEB-9C68-D17EDDB9AB1A}" name="VARIABLE"/>
     <tableColumn id="2" xr3:uid="{F3934D33-F0E4-4E5F-82F5-09C1B54B6EB5}" name="UNIT OF MEASURE"/>
     <tableColumn id="3" xr3:uid="{1F404554-AF31-420E-AFBD-07C7BC574AF4}" name="DESCRIPTION"/>
-    <tableColumn id="4" xr3:uid="{FBF9B961-94BF-4C83-A187-FFF4CC755D65}" name="CLASSES" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FBF9B961-94BF-4C83-A187-FFF4CC755D65}" name="CLASSES" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7476CB9C-69BD-436C-92EA-B35C4849E91C}" name="Tabella4" displayName="Tabella4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7476CB9C-69BD-436C-92EA-B35C4849E91C}" name="Tabella4" displayName="Tabella4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:D4" xr:uid="{7476CB9C-69BD-436C-92EA-B35C4849E91C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A3EB4BDB-FFB4-4696-8AA9-BE567875F256}" name="VARIABLE"/>
     <tableColumn id="2" xr3:uid="{1A3ABF46-D8A9-4088-BC58-E26C73C06451}" name="UNIT OF MEASURE"/>
     <tableColumn id="3" xr3:uid="{17AE67B3-B7B0-42B2-B43A-2E2CC0605242}" name="DESCRIPTION"/>
-    <tableColumn id="4" xr3:uid="{76BEE7E0-8D0D-43BE-AFAC-EE77E8472FC0}" name="CLASSES" dataDxfId="2" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" xr3:uid="{76BEE7E0-8D0D-43BE-AFAC-EE77E8472FC0}" name="CLASSES" dataDxfId="1" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED8FAC1-F10A-4C33-9F47-7BA340A4C1B2}" name="Tabella1" displayName="Tabella1" ref="A1:D20" totalsRowShown="0">
-  <autoFilter ref="A1:D20" xr:uid="{3ED8FAC1-F10A-4C33-9F47-7BA340A4C1B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED8FAC1-F10A-4C33-9F47-7BA340A4C1B2}" name="Tabella1" displayName="Tabella1" ref="A1:D23" totalsRowShown="0">
+  <autoFilter ref="A1:D23" xr:uid="{3ED8FAC1-F10A-4C33-9F47-7BA340A4C1B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C9E63D5A-2AE5-4D31-AEB8-EB047A90BD1D}" name="VARIABLE"/>
     <tableColumn id="2" xr3:uid="{8FC6B31D-B5C3-45C7-8E02-A9003AC4AA5A}" name="UNIT OF MEASURE"/>
@@ -1659,8 +1691,8 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1682,7 +1714,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1810,6 +1842,9 @@
       <c r="C11" t="s">
         <v>307</v>
       </c>
+      <c r="D11" t="s">
+        <v>350</v>
+      </c>
       <c r="F11" t="s">
         <v>321</v>
       </c>
@@ -1932,6 +1967,9 @@
       <c r="A21" t="s">
         <v>282</v>
       </c>
+      <c r="B21" t="s">
+        <v>294</v>
+      </c>
       <c r="C21" t="s">
         <v>315</v>
       </c>
@@ -1940,6 +1978,9 @@
       <c r="A22" t="s">
         <v>283</v>
       </c>
+      <c r="B22" t="s">
+        <v>294</v>
+      </c>
       <c r="C22" t="s">
         <v>314</v>
       </c>
@@ -1951,7 +1992,7 @@
       <c r="B23" t="s">
         <v>294</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>316</v>
       </c>
     </row>
@@ -3876,17 +3917,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042C54E9-CF20-4A13-A407-7E56CCAD825C}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="124.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3926,191 +3967,233 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>341</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>340</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>341</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>343</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>344</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>345</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>347</v>
+      </c>
+      <c r="D18" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>